<commit_message>
Modified multi-level output per-core width and added arbiter input padding
</commit_message>
<xml_diff>
--- a/die_info.xlsx
+++ b/die_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weier Wan\Dropbox\neurram\48_core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F7A37C-81E5-43C5-BBA7-395C04FEA511}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634FE830-E32B-4554-89EA-34DDD37714F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2655" yWindow="390" windowWidth="21660" windowHeight="15120" xr2:uid="{570F0E5D-8F67-4062-BD0B-BB95E9155A55}"/>
+    <workbookView xWindow="33930" yWindow="6885" windowWidth="21600" windowHeight="11385" xr2:uid="{570F0E5D-8F67-4062-BD0B-BB95E9155A55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t># chip</t>
   </si>
@@ -65,12 +65,6 @@
     <t>97, 117, 132, 165, 181, 241</t>
   </si>
   <si>
-    <t>1, 17, 19, 25, 26, 65, 68, 69, 80, 96, 105, 127, 130, 147, 148, 149, 164, 166, 188, 210, 217, 221, 229, 239, 248</t>
-  </si>
-  <si>
-    <t>27, 29, 32, 49, 51, 53, 68, 84, 91, 113, 114, 116, 118, 129, 131, 137, 140, 164, 170, 176, 196, 206, 210, 214, 217, 234, 241, 243, 251, 255</t>
-  </si>
-  <si>
     <t>115,</t>
   </si>
   <si>
@@ -99,16 +93,89 @@
   </si>
   <si>
     <t>100, 244</t>
+  </si>
+  <si>
+    <t>13, 67, 187</t>
+  </si>
+  <si>
+    <t>0, 6, 10, 22, 23, 29, 34, 35, 42, 46, 48, 50, 52, 53, 57, 66, 73, 74, 80, 82, 85, 88, 89, 90, 92, 95, 96, 99, 103, 117, 118, 119, 120, 121, 126, 128, 131, 142, 150, 158, 160, 163, 166, 169, 173, 178, 179, 188, 191, 192, 209, 210, 213, 219, 228, 231, 236, 238, 240, 241, 244, 246, 255</t>
+  </si>
+  <si>
+    <t>15, 32, 230</t>
+  </si>
+  <si>
+    <t>10, 12, 13, 21, 26, 36, 42, 43, 44, 52, 53, 68, 83, 95, 103, 108, 109, 112, 114, 121, 122, 127, 134, 138, 147, 148, 167, 168, 169, 180, 186, 193, 210, 211, 214, 215, 228, 240, 241</t>
+  </si>
+  <si>
+    <t>34, 43, 45, 50, 52, 57, 60, 71, 73, 82, 86, 87, 101, 112, 117, 118, 126, 128, 130, 142, 144, 148, 150, 160, 164, 166, 177, 183, 185, 190, 192, 198, 201, 202, 203, 210, 212, 214, 218, 220, 226, 227, 236, 249, 252</t>
+  </si>
+  <si>
+    <t>149, 244, 247</t>
+  </si>
+  <si>
+    <t>167,</t>
+  </si>
+  <si>
+    <t>1, 17, 19, 25, 26, 65, 68, 69, 80, 96, 105, 127, 130, 147, 148, 149, 164, 166, 188, 210, 217, 221, 229, 239, 248, 20</t>
+  </si>
+  <si>
+    <t>27, 29, 32, 49, 51, 53, 68, 84, 91, 113, 114, 116, 118, 129, 131, 137, 140, 164, 170, 176, 196, 206, 210, 214, 217, 234, 241, 243, 251, 255, 0, 160</t>
+  </si>
+  <si>
+    <t>18, 19, 27, 51, 63, 66, 76, 87, 100, 123, 132, 149, 152, 165, 169, 171, 178, 191, 198, 207, 208, 209, 213, 216, 222, 237, 245</t>
+  </si>
+  <si>
+    <t>too many unformed</t>
+  </si>
+  <si>
+    <t>6, 14, 22, 25, 26, 31, 33, 35, 43, 45, 52, 60, 62, 65, 103, 105, 106, 107, 112, 113, 122, 124, 127, 140, 142, 146, 150, 152, 154, 155, 159, 165, 167, 177, 178, 181, 184, 185, 190, 192, 203, 204, 212, 214, 217, 219, 225, 228, 229, 233, 246, 247, 251</t>
+  </si>
+  <si>
+    <t>86, 163</t>
+  </si>
+  <si>
+    <t>34,</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6, 13, 15, 25, 44, 51, 56, 61, 82, 101, 109, 116, 133, 165, 168, 176, 181, 184, 192, 196, 198, 219, 222, 223, 232, 235, 239, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>250</t>
+    </r>
+  </si>
+  <si>
+    <t>22, 28, 29, 31, 41, 51, 61, 79, 85, 91, 105, 108, 122, 129, 139, 144, 153, 164, 167, 187, 199, 201, 218, 226, 230, 233, 235, 252, 254, 14, 26</t>
+  </si>
+  <si>
+    <t>2, 11, 14, 43, 57, 58, 60, 73, 80, 98, 100, 101, 112, 113, 133, 156, 161, 166, 173, 175, 184, 187, 217, 233, 240, 245, 255</t>
+  </si>
+  <si>
+    <t>unformed columns</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,8 +201,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -456,29 +529,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749E0D37-CBA6-4D65-800C-C66E3749780F}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="116.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="5" max="6" width="30.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -487,17 +560,20 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>0</v>
       </c>
       <c r="C2" s="1">
@@ -507,15 +583,15 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2">
+        <v>13</v>
+      </c>
+      <c r="H2">
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="1">
         <v>1</v>
       </c>
@@ -525,13 +601,13 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="1">
         <v>2</v>
       </c>
@@ -541,123 +617,283 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="1">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="G5">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="H5">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="1">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="1">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7">
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4">
         <v>1</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8">
+        <v>16</v>
+      </c>
+      <c r="H8">
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="1">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9">
+        <v>19</v>
+      </c>
+      <c r="H9">
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="1">
         <v>5</v>
       </c>
     </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>15</v>
+      </c>
+      <c r="H14">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="1">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="A14:A25"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B14:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>